<commit_message>
before possible breaking changes to fetchPricingData function
</commit_message>
<xml_diff>
--- a/isinData/isinData.xlsx
+++ b/isinData/isinData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/baltiearaneta/Documents/Coding/Projects/BPI App/server/isinData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EFC66F5-13B4-7C46-8294-3AB43E9BC954}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AFD9E0C-1328-B949-B9B0-FE6539CB8756}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14400" yWindow="500" windowWidth="14400" windowHeight="16400" xr2:uid="{2E953191-0F9A-B142-86F2-92A04FF2A3EB}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
   <si>
     <t>5-77</t>
   </si>
@@ -109,6 +109,15 @@
   </si>
   <si>
     <t>PIBD1031G662</t>
+  </si>
+  <si>
+    <t>PIBD0726B627</t>
+  </si>
+  <si>
+    <t>7-62</t>
+  </si>
+  <si>
+    <t>762</t>
   </si>
 </sst>
 </file>
@@ -477,10 +486,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3EA1D06-52FD-B240-B560-F7529C9097EF}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -615,6 +624,20 @@
         <v>11526</v>
       </c>
     </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="6">
+        <v>46067</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
uploading time and sales
</commit_message>
<xml_diff>
--- a/isinData/isinData.xlsx
+++ b/isinData/isinData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/baltiearaneta/Documents/Coding/Projects/BPI App/server/isinData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9471204E-413E-634A-8737-450B915A1836}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AE406CD-FD74-BC47-9A21-6216785C2618}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14400" yWindow="500" windowWidth="14400" windowHeight="16400" xr2:uid="{2E953191-0F9A-B142-86F2-92A04FF2A3EB}"/>
   </bookViews>
@@ -495,7 +495,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
nov 17 afternoon, notifications
</commit_message>
<xml_diff>
--- a/isinData/isinData.xlsx
+++ b/isinData/isinData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/baltiearaneta/Documents/Coding/Projects/BPI App/server/isinData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5179BB0-F713-684B-9903-4A21EEB96A75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B27AC918-EFB1-D94B-B9DB-09D8E8D7CD28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="14400" windowHeight="16440" xr2:uid="{2E953191-0F9A-B142-86F2-92A04FF2A3EB}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="14400" windowHeight="16420" xr2:uid="{2E953191-0F9A-B142-86F2-92A04FF2A3EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="267">
   <si>
     <t>5-77</t>
   </si>
@@ -633,36 +633,9 @@
     <t>11/16/22</t>
   </si>
   <si>
-    <t>05-11</t>
-  </si>
-  <si>
-    <t>03-10</t>
-  </si>
-  <si>
-    <t>10-04</t>
-  </si>
-  <si>
-    <t>05-12</t>
-  </si>
-  <si>
-    <t>05-13</t>
-  </si>
-  <si>
-    <t>25-01</t>
-  </si>
-  <si>
     <t>10-05</t>
   </si>
   <si>
-    <t>15-01</t>
-  </si>
-  <si>
-    <t>15-02</t>
-  </si>
-  <si>
-    <t>20-01</t>
-  </si>
-  <si>
     <t>574</t>
   </si>
   <si>
@@ -699,9 +672,6 @@
     <t>2501</t>
   </si>
   <si>
-    <t>03-11</t>
-  </si>
-  <si>
     <t>0574</t>
   </si>
   <si>
@@ -841,6 +811,30 @@
   </si>
   <si>
     <t>watchlist</t>
+  </si>
+  <si>
+    <t>R512</t>
+  </si>
+  <si>
+    <t>R104</t>
+  </si>
+  <si>
+    <t>R310</t>
+  </si>
+  <si>
+    <t>R511</t>
+  </si>
+  <si>
+    <t>R201</t>
+  </si>
+  <si>
+    <t>R251</t>
+  </si>
+  <si>
+    <t>R152</t>
+  </si>
+  <si>
+    <t>R151</t>
   </si>
 </sst>
 </file>
@@ -1210,10 +1204,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3EA1D06-52FD-B240-B560-F7529C9097EF}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:E131"/>
+  <dimension ref="A1:E129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A107" workbookViewId="0">
-      <selection activeCell="C115" sqref="A115:XFD115"/>
+    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="D73" sqref="D73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1236,7 +1230,7 @@
         <v>20</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>268</v>
+        <v>258</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -1421,10 +1415,10 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="C14" t="s">
         <v>42</v>
@@ -1799,10 +1793,10 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="C39" t="s">
         <v>67</v>
@@ -1877,7 +1871,7 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="C44" t="s">
         <v>72</v>
@@ -1982,7 +1976,7 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="C51" t="s">
         <v>79</v>
@@ -2072,7 +2066,7 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="C57" t="s">
         <v>85</v>
@@ -2162,10 +2156,10 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
-        <v>199</v>
+        <v>262</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="C63" t="s">
         <v>91</v>
@@ -2180,7 +2174,7 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="C64" t="s">
         <v>92</v>
@@ -2195,10 +2189,10 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
-        <v>200</v>
+        <v>261</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>267</v>
+        <v>257</v>
       </c>
       <c r="C65" t="s">
         <v>93</v>
@@ -2213,7 +2207,7 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" s="3" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
       <c r="C66" t="s">
         <v>94</v>
@@ -2228,7 +2222,7 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" s="3" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="C67" t="s">
         <v>95</v>
@@ -2243,7 +2237,7 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" s="3" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="C68" t="s">
         <v>96</v>
@@ -2258,7 +2252,7 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" s="3" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="C69" t="s">
         <v>97</v>
@@ -2273,10 +2267,10 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" s="3" t="s">
-        <v>201</v>
+        <v>260</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="C70" t="s">
         <v>98</v>
@@ -2291,7 +2285,7 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" s="3" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="C71" t="s">
         <v>99</v>
@@ -2306,7 +2300,7 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" s="3" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="C72" t="s">
         <v>100</v>
@@ -2339,16 +2333,16 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" s="3" t="s">
-        <v>221</v>
+        <v>259</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>214</v>
+        <v>256</v>
       </c>
       <c r="C74" t="s">
-        <v>9</v>
+        <v>101</v>
       </c>
       <c r="D74" s="6">
-        <v>45360</v>
+        <v>45363</v>
       </c>
       <c r="E74" t="b">
         <f>FALSE</f>
@@ -2357,16 +2351,13 @@
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" s="3" t="s">
-        <v>202</v>
-      </c>
-      <c r="B75" s="3" t="s">
-        <v>266</v>
+        <v>219</v>
       </c>
       <c r="C75" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D75" s="6">
-        <v>45363</v>
+        <v>45402</v>
       </c>
       <c r="E75" t="b">
         <f>FALSE</f>
@@ -2375,13 +2366,13 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" s="3" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
       <c r="C76" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D76" s="6">
-        <v>45402</v>
+        <v>45446</v>
       </c>
       <c r="E76" t="b">
         <f>FALSE</f>
@@ -2390,13 +2381,13 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" s="3" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
       <c r="C77" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D77" s="6">
-        <v>45446</v>
+        <v>45509</v>
       </c>
       <c r="E77" t="b">
         <f>FALSE</f>
@@ -2405,13 +2396,13 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" s="3" t="s">
-        <v>231</v>
+        <v>222</v>
       </c>
       <c r="C78" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D78" s="6">
-        <v>45509</v>
+        <v>45524</v>
       </c>
       <c r="E78" t="b">
         <f>FALSE</f>
@@ -2420,13 +2411,13 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" s="3" t="s">
-        <v>232</v>
+        <v>223</v>
       </c>
       <c r="C79" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D79" s="6">
-        <v>45524</v>
+        <v>45582</v>
       </c>
       <c r="E79" t="b">
         <f>FALSE</f>
@@ -2435,13 +2426,13 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" s="3" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="C80" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D80" s="6">
-        <v>45582</v>
+        <v>45607</v>
       </c>
       <c r="E80" t="b">
         <f>FALSE</f>
@@ -2450,13 +2441,13 @@
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" s="3" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="C81" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D81" s="6">
-        <v>45607</v>
+        <v>45759</v>
       </c>
       <c r="E81" t="b">
         <f>FALSE</f>
@@ -2465,13 +2456,13 @@
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" s="3" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="C82" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D82" s="6">
-        <v>45759</v>
+        <v>45761</v>
       </c>
       <c r="E82" t="b">
         <f>FALSE</f>
@@ -2479,32 +2470,35 @@
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A83" s="3" t="s">
-        <v>236</v>
+      <c r="A83" t="s">
+        <v>3</v>
+      </c>
+      <c r="B83" s="3" t="s">
+        <v>4</v>
       </c>
       <c r="C83" t="s">
-        <v>109</v>
-      </c>
-      <c r="D83" s="6">
-        <v>45761</v>
+        <v>12</v>
+      </c>
+      <c r="D83" s="5">
+        <v>45881</v>
       </c>
       <c r="E83" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <f>TRUE</f>
+        <v>1</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A84" t="s">
-        <v>3</v>
+      <c r="A84" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="C84" t="s">
-        <v>12</v>
-      </c>
-      <c r="D84" s="5">
-        <v>45881</v>
+        <v>29</v>
+      </c>
+      <c r="D84" s="6">
+        <v>45909</v>
       </c>
       <c r="E84" t="b">
         <f>TRUE</f>
@@ -2513,13 +2507,13 @@
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" s="3" t="s">
-        <v>203</v>
+        <v>227</v>
       </c>
       <c r="C85" t="s">
-        <v>12</v>
+        <v>110</v>
       </c>
       <c r="D85" s="6">
-        <v>45881</v>
+        <v>45950</v>
       </c>
       <c r="E85" t="b">
         <f>FALSE</f>
@@ -2528,61 +2522,61 @@
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B86" s="3" t="s">
-        <v>28</v>
+        <v>211</v>
       </c>
       <c r="C86" t="s">
-        <v>29</v>
+        <v>111</v>
       </c>
       <c r="D86" s="6">
-        <v>45909</v>
+        <v>45990</v>
       </c>
       <c r="E86" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A87" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="C87" t="s">
+        <v>112</v>
+      </c>
+      <c r="D87" s="6">
+        <v>46041</v>
+      </c>
+      <c r="E87" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A88" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B88" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C88" t="s">
+        <v>25</v>
+      </c>
+      <c r="D88" s="6">
+        <v>46067</v>
+      </c>
+      <c r="E88" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A87" s="3" t="s">
-        <v>237</v>
-      </c>
-      <c r="C87" t="s">
-        <v>110</v>
-      </c>
-      <c r="D87" s="6">
-        <v>45950</v>
-      </c>
-      <c r="E87" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A88" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="C88" t="s">
-        <v>111</v>
-      </c>
-      <c r="D88" s="6">
-        <v>45990</v>
-      </c>
-      <c r="E88" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89" s="3" t="s">
-        <v>238</v>
+        <v>229</v>
       </c>
       <c r="C89" t="s">
-        <v>112</v>
+        <v>25</v>
       </c>
       <c r="D89" s="6">
-        <v>46041</v>
+        <v>46067</v>
       </c>
       <c r="E89" t="b">
         <f>FALSE</f>
@@ -2591,16 +2585,16 @@
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90" s="2" t="s">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>27</v>
+        <v>2</v>
       </c>
       <c r="C90" t="s">
-        <v>25</v>
-      </c>
-      <c r="D90" s="6">
-        <v>46067</v>
+        <v>7</v>
+      </c>
+      <c r="D90" s="5">
+        <v>46120</v>
       </c>
       <c r="E90" t="b">
         <f>TRUE</f>
@@ -2609,13 +2603,13 @@
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91" s="3" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="C91" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="D91" s="6">
-        <v>46067</v>
+        <v>46120</v>
       </c>
       <c r="E91" t="b">
         <f>FALSE</f>
@@ -2623,95 +2617,95 @@
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A92" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B92" s="3" t="s">
-        <v>2</v>
+      <c r="A92" s="3" t="s">
+        <v>199</v>
       </c>
       <c r="C92" t="s">
-        <v>7</v>
-      </c>
-      <c r="D92" s="5">
-        <v>46120</v>
+        <v>113</v>
+      </c>
+      <c r="D92" s="6">
+        <v>46285</v>
       </c>
       <c r="E92" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A93" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="C93" t="s">
+        <v>114</v>
+      </c>
+      <c r="D93" s="6">
+        <v>46315</v>
+      </c>
+      <c r="E93" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A94" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="C94" t="s">
+        <v>115</v>
+      </c>
+      <c r="D94" s="6">
+        <v>46363</v>
+      </c>
+      <c r="E94" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A95" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="B95" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="C95" t="s">
+        <v>116</v>
+      </c>
+      <c r="D95" s="6">
+        <v>46447</v>
+      </c>
+      <c r="E95" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A96" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B96" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C96" t="s">
+        <v>8</v>
+      </c>
+      <c r="D96" s="5">
+        <v>46511</v>
+      </c>
+      <c r="E96" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A93" s="3" t="s">
-        <v>240</v>
-      </c>
-      <c r="C93" t="s">
-        <v>7</v>
-      </c>
-      <c r="D93" s="6">
-        <v>46120</v>
-      </c>
-      <c r="E93" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A94" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="C94" t="s">
-        <v>113</v>
-      </c>
-      <c r="D94" s="6">
-        <v>46285</v>
-      </c>
-      <c r="E94" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A95" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="C95" t="s">
-        <v>114</v>
-      </c>
-      <c r="D95" s="6">
-        <v>46315</v>
-      </c>
-      <c r="E95" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A96" s="3" t="s">
-        <v>241</v>
-      </c>
-      <c r="C96" t="s">
-        <v>115</v>
-      </c>
-      <c r="D96" s="6">
-        <v>46363</v>
-      </c>
-      <c r="E96" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="B97" s="3" t="s">
-        <v>218</v>
+        <v>1</v>
       </c>
       <c r="C97" t="s">
-        <v>116</v>
+        <v>8</v>
       </c>
       <c r="D97" s="6">
-        <v>46447</v>
+        <v>46511</v>
       </c>
       <c r="E97" t="b">
         <f>FALSE</f>
@@ -2720,61 +2714,61 @@
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A98" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B98" s="3" t="s">
-        <v>1</v>
+        <v>232</v>
       </c>
       <c r="C98" t="s">
-        <v>8</v>
-      </c>
-      <c r="D98" s="5">
-        <v>46511</v>
+        <v>117</v>
+      </c>
+      <c r="D98" s="6">
+        <v>46636</v>
       </c>
       <c r="E98" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A99" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="C99" t="s">
+        <v>118</v>
+      </c>
+      <c r="D99" s="6">
+        <v>46834</v>
+      </c>
+      <c r="E99" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A100" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B100" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C100" t="s">
+        <v>16</v>
+      </c>
+      <c r="D100" s="6">
+        <v>46865</v>
+      </c>
+      <c r="E100" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A99" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C99" t="s">
-        <v>8</v>
-      </c>
-      <c r="D99" s="6">
-        <v>46511</v>
-      </c>
-      <c r="E99" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A100" s="3" t="s">
-        <v>242</v>
-      </c>
-      <c r="C100" t="s">
-        <v>117</v>
-      </c>
-      <c r="D100" s="6">
-        <v>46636</v>
-      </c>
-      <c r="E100" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A101" s="3" t="s">
-        <v>243</v>
+        <v>234</v>
       </c>
       <c r="C101" t="s">
-        <v>118</v>
+        <v>16</v>
       </c>
       <c r="D101" s="6">
-        <v>46834</v>
+        <v>46865</v>
       </c>
       <c r="E101" t="b">
         <f>FALSE</f>
@@ -2782,17 +2776,17 @@
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A102" s="2" t="s">
-        <v>14</v>
+      <c r="A102" s="3" t="s">
+        <v>18</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C102" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D102" s="6">
-        <v>46865</v>
+        <v>46977</v>
       </c>
       <c r="E102" t="b">
         <f>TRUE</f>
@@ -2801,13 +2795,13 @@
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A103" s="3" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
       <c r="C103" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D103" s="6">
-        <v>46865</v>
+        <v>46977</v>
       </c>
       <c r="E103" t="b">
         <f>FALSE</f>
@@ -2816,76 +2810,76 @@
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A104" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B104" s="3" t="s">
-        <v>19</v>
+        <v>236</v>
       </c>
       <c r="C104" t="s">
-        <v>17</v>
+        <v>119</v>
       </c>
       <c r="D104" s="6">
-        <v>46977</v>
+        <v>47091</v>
       </c>
       <c r="E104" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A105" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="C105" t="s">
+        <v>120</v>
+      </c>
+      <c r="D105" s="6">
+        <v>47128</v>
+      </c>
+      <c r="E105" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A106" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="C106" t="s">
+        <v>121</v>
+      </c>
+      <c r="D106" s="6">
+        <v>47630</v>
+      </c>
+      <c r="E106" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A107" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B107" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C107" t="s">
+        <v>22</v>
+      </c>
+      <c r="D107" s="6">
+        <v>47673</v>
+      </c>
+      <c r="E107" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A105" s="3" t="s">
-        <v>245</v>
-      </c>
-      <c r="C105" t="s">
-        <v>17</v>
-      </c>
-      <c r="D105" s="6">
-        <v>46977</v>
-      </c>
-      <c r="E105" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A106" s="3" t="s">
-        <v>246</v>
-      </c>
-      <c r="C106" t="s">
-        <v>119</v>
-      </c>
-      <c r="D106" s="6">
-        <v>47091</v>
-      </c>
-      <c r="E106" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A107" s="3" t="s">
-        <v>247</v>
-      </c>
-      <c r="C107" t="s">
-        <v>120</v>
-      </c>
-      <c r="D107" s="6">
-        <v>47128</v>
-      </c>
-      <c r="E107" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A108" s="3" t="s">
-        <v>248</v>
+        <v>23</v>
       </c>
       <c r="C108" t="s">
-        <v>121</v>
+        <v>22</v>
       </c>
       <c r="D108" s="6">
-        <v>47630</v>
+        <v>47673</v>
       </c>
       <c r="E108" t="b">
         <f>FALSE</f>
@@ -2894,76 +2888,76 @@
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A109" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B109" s="3" t="s">
-        <v>23</v>
+        <v>239</v>
       </c>
       <c r="C109" t="s">
-        <v>22</v>
+        <v>122</v>
       </c>
       <c r="D109" s="6">
-        <v>47673</v>
+        <v>47692</v>
       </c>
       <c r="E109" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A110" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="C110" t="s">
+        <v>123</v>
+      </c>
+      <c r="D110" s="6">
+        <v>47874</v>
+      </c>
+      <c r="E110" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A111" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="C111" t="s">
+        <v>124</v>
+      </c>
+      <c r="D111" s="6">
+        <v>48048</v>
+      </c>
+      <c r="E111" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A112" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B112" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C112" t="s">
+        <v>24</v>
+      </c>
+      <c r="D112" s="6">
+        <v>48051</v>
+      </c>
+      <c r="E112" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A110" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C110" t="s">
-        <v>22</v>
-      </c>
-      <c r="D110" s="6">
-        <v>47673</v>
-      </c>
-      <c r="E110" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A111" s="3" t="s">
-        <v>249</v>
-      </c>
-      <c r="C111" t="s">
-        <v>122</v>
-      </c>
-      <c r="D111" s="6">
-        <v>47692</v>
-      </c>
-      <c r="E111" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A112" s="3" t="s">
-        <v>250</v>
-      </c>
-      <c r="C112" t="s">
-        <v>123</v>
-      </c>
-      <c r="D112" s="6">
-        <v>47874</v>
-      </c>
-      <c r="E112" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A113" s="3" t="s">
-        <v>251</v>
+        <v>242</v>
       </c>
       <c r="C113" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D113" s="6">
-        <v>48048</v>
+        <v>48126</v>
       </c>
       <c r="E113" t="b">
         <f>FALSE</f>
@@ -2972,31 +2966,31 @@
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A114" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B114" s="3" t="s">
-        <v>21</v>
+        <v>243</v>
       </c>
       <c r="C114" t="s">
-        <v>24</v>
+        <v>126</v>
       </c>
       <c r="D114" s="6">
-        <v>48051</v>
+        <v>48246</v>
       </c>
       <c r="E114" t="b">
-        <f>TRUE</f>
-        <v>1</v>
+        <f>FALSE</f>
+        <v>0</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A115" s="3" t="s">
-        <v>252</v>
+        <v>263</v>
+      </c>
+      <c r="B115" s="3" t="s">
+        <v>210</v>
       </c>
       <c r="C115" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="D115" s="6">
-        <v>48126</v>
+        <v>48274</v>
       </c>
       <c r="E115" t="b">
         <f>FALSE</f>
@@ -3005,13 +2999,13 @@
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A116" s="3" t="s">
-        <v>253</v>
+        <v>244</v>
       </c>
       <c r="C116" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="D116" s="6">
-        <v>48246</v>
+        <v>48484</v>
       </c>
       <c r="E116" t="b">
         <f>FALSE</f>
@@ -3020,16 +3014,13 @@
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A117" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="B117" s="3" t="s">
-        <v>219</v>
+        <v>245</v>
       </c>
       <c r="C117" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="D117" s="6">
-        <v>48274</v>
+        <v>48547</v>
       </c>
       <c r="E117" t="b">
         <f>FALSE</f>
@@ -3038,13 +3029,13 @@
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A118" s="3" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="C118" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="D118" s="6">
-        <v>48484</v>
+        <v>48659</v>
       </c>
       <c r="E118" t="b">
         <f>FALSE</f>
@@ -3053,13 +3044,13 @@
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A119" s="3" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="C119" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="D119" s="6">
-        <v>48547</v>
+        <v>49253</v>
       </c>
       <c r="E119" t="b">
         <f>FALSE</f>
@@ -3068,13 +3059,13 @@
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A120" s="3" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="C120" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="D120" s="6">
-        <v>48659</v>
+        <v>49582</v>
       </c>
       <c r="E120" t="b">
         <f>FALSE</f>
@@ -3083,13 +3074,13 @@
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A121" s="3" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="C121" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="D121" s="6">
-        <v>49253</v>
+        <v>49659</v>
       </c>
       <c r="E121" t="b">
         <f>FALSE</f>
@@ -3098,13 +3089,13 @@
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A122" s="3" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="C122" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D122" s="6">
-        <v>49582</v>
+        <v>49947</v>
       </c>
       <c r="E122" t="b">
         <f>FALSE</f>
@@ -3113,13 +3104,13 @@
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A123" s="3" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="C123" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="D123" s="6">
-        <v>49659</v>
+        <v>50178</v>
       </c>
       <c r="E123" t="b">
         <f>FALSE</f>
@@ -3128,13 +3119,13 @@
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A124" s="3" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
       <c r="C124" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="D124" s="6">
-        <v>49947</v>
+        <v>50268</v>
       </c>
       <c r="E124" t="b">
         <f>FALSE</f>
@@ -3143,13 +3134,16 @@
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A125" s="3" t="s">
-        <v>261</v>
+        <v>264</v>
+      </c>
+      <c r="B125" s="3" t="s">
+        <v>211</v>
       </c>
       <c r="C125" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="D125" s="6">
-        <v>50178</v>
+        <v>50337</v>
       </c>
       <c r="E125" t="b">
         <f>FALSE</f>
@@ -3158,13 +3152,13 @@
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A126" s="3" t="s">
-        <v>262</v>
+        <v>253</v>
       </c>
       <c r="C126" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="D126" s="6">
-        <v>50268</v>
+        <v>50458</v>
       </c>
       <c r="E126" t="b">
         <f>FALSE</f>
@@ -3173,16 +3167,13 @@
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A127" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="B127" s="3" t="s">
-        <v>220</v>
+        <v>254</v>
       </c>
       <c r="C127" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="D127" s="6">
-        <v>50337</v>
+        <v>50794</v>
       </c>
       <c r="E127" t="b">
         <f>FALSE</f>
@@ -3191,13 +3182,13 @@
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A128" s="3" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="C128" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="D128" s="6">
-        <v>50458</v>
+        <v>51388</v>
       </c>
       <c r="E128" t="b">
         <f>FALSE</f>
@@ -3206,52 +3197,22 @@
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A129" s="3" t="s">
-        <v>264</v>
+        <v>145</v>
       </c>
       <c r="C129" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="D129" s="6">
-        <v>50794</v>
+        <v>51697</v>
       </c>
       <c r="E129" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A130" s="3" t="s">
-        <v>265</v>
-      </c>
-      <c r="C130" t="s">
-        <v>140</v>
-      </c>
-      <c r="D130" s="6">
-        <v>51388</v>
-      </c>
-      <c r="E130" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A131" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="C131" t="s">
-        <v>141</v>
-      </c>
-      <c r="D131" s="6">
-        <v>51697</v>
-      </c>
-      <c r="E131" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D131">
-    <sortCondition ref="D2:D131"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D129">
+    <sortCondition ref="D2:D129"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
dec 2 afternoon changes
</commit_message>
<xml_diff>
--- a/isinData/isinData.xlsx
+++ b/isinData/isinData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/baltiearaneta/Documents/Coding/Projects/BPI App/server/isinData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AE0C978-4E6F-2648-94AE-42A1F73E3689}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B20CD719-586D-BE41-A15E-A12ABEA74390}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="14400" windowHeight="16380" xr2:uid="{2E953191-0F9A-B142-86F2-92A04FF2A3EB}"/>
+    <workbookView xWindow="14400" yWindow="500" windowWidth="14400" windowHeight="16360" xr2:uid="{2E953191-0F9A-B142-86F2-92A04FF2A3EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="270">
   <si>
     <t>5-77</t>
   </si>
@@ -835,6 +835,15 @@
   </si>
   <si>
     <t>R151</t>
+  </si>
+  <si>
+    <t>R514</t>
+  </si>
+  <si>
+    <t>PIID0527L140</t>
+  </si>
+  <si>
+    <t>514</t>
   </si>
 </sst>
 </file>
@@ -1206,8 +1215,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:E129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="C75" sqref="C75"/>
+    <sheetView tabSelected="1" topLeftCell="A90" workbookViewId="0">
+      <selection activeCell="A97" sqref="A97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2699,17 +2708,19 @@
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="B97" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="C97" t="s">
+        <v>268</v>
+      </c>
+      <c r="D97" s="6">
+        <v>46540</v>
+      </c>
+      <c r="E97" t="b">
         <v>1</v>
-      </c>
-      <c r="C97" t="s">
-        <v>8</v>
-      </c>
-      <c r="D97" s="6">
-        <v>46511</v>
-      </c>
-      <c r="E97" t="b">
-        <f>FALSE</f>
-        <v>0</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
time and sales updates
</commit_message>
<xml_diff>
--- a/isinData/isinData.xlsx
+++ b/isinData/isinData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/baltiearaneta/Documents/Coding/Projects/BPI App/server/isinData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A25D532-881A-7240-B4CA-75848E319FC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F650900-B065-0843-9459-3844EFFA266E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="14400" windowHeight="16380" xr2:uid="{2E953191-0F9A-B142-86F2-92A04FF2A3EB}"/>
+    <workbookView xWindow="14400" yWindow="500" windowWidth="14400" windowHeight="16380" xr2:uid="{2E953191-0F9A-B142-86F2-92A04FF2A3EB}"/>
   </bookViews>
   <sheets>
     <sheet name="List" sheetId="3" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2151" uniqueCount="423">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2154" uniqueCount="425">
   <si>
     <t>5-77</t>
   </si>
@@ -1304,6 +1304,12 @@
   </si>
   <si>
     <t>PIBL1222A013</t>
+  </si>
+  <si>
+    <t>01/11/23</t>
+  </si>
+  <si>
+    <t>PIBL1222A022</t>
   </si>
 </sst>
 </file>
@@ -1659,13 +1665,16 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27B9CCD1-6E22-9748-BFF1-8181B4AF161F}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:G123"/>
+  <dimension ref="A1:G124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A102" workbookViewId="0">
-      <selection activeCell="D98" sqref="D98"/>
+    <sheetView tabSelected="1" topLeftCell="A116" workbookViewId="0">
+      <selection activeCell="C123" sqref="C123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -2943,42 +2952,43 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>228</v>
+        <v>423</v>
       </c>
       <c r="C64" t="s">
-        <v>86</v>
-      </c>
-      <c r="D64">
-        <v>4.375</v>
+        <v>424</v>
+      </c>
+      <c r="D64" t="s">
+        <v>268</v>
       </c>
       <c r="E64" s="2">
-        <v>43872</v>
+        <v>44573</v>
       </c>
       <c r="F64" s="2">
-        <v>44968</v>
+        <v>44937</v>
       </c>
       <c r="G64" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>194</v>
+        <v>232</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>228</v>
       </c>
       <c r="C65" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D65">
-        <v>13</v>
+        <v>4.375</v>
       </c>
       <c r="E65" s="2">
-        <v>37672</v>
+        <v>43872</v>
       </c>
       <c r="F65" s="2">
-        <v>44977</v>
+        <v>44968</v>
       </c>
       <c r="G65" t="b">
         <v>0</v>
@@ -2986,22 +2996,19 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>406</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>393</v>
+        <v>194</v>
       </c>
       <c r="C66" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D66">
-        <v>5.5</v>
+        <v>13</v>
       </c>
       <c r="E66" s="2">
-        <v>43167</v>
+        <v>37672</v>
       </c>
       <c r="F66" s="2">
-        <v>44993</v>
+        <v>44977</v>
       </c>
       <c r="G66" t="b">
         <v>0</v>
@@ -3009,22 +3016,22 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>408</v>
+        <v>393</v>
       </c>
       <c r="C67" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D67">
-        <v>3.5</v>
+        <v>5.5</v>
       </c>
       <c r="E67" s="2">
-        <v>42481</v>
+        <v>43167</v>
       </c>
       <c r="F67" s="2">
-        <v>45037</v>
+        <v>44993</v>
       </c>
       <c r="G67" t="b">
         <v>0</v>
@@ -3032,19 +3039,22 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>195</v>
+        <v>407</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>408</v>
       </c>
       <c r="C68" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D68">
-        <v>11.875</v>
+        <v>3.5</v>
       </c>
       <c r="E68" s="2">
-        <v>37770</v>
+        <v>42481</v>
       </c>
       <c r="F68" s="2">
-        <v>45075</v>
+        <v>45037</v>
       </c>
       <c r="G68" t="b">
         <v>0</v>
@@ -3052,22 +3062,19 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>409</v>
+        <v>195</v>
       </c>
       <c r="C69" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D69">
-        <v>3.25</v>
+        <v>11.875</v>
       </c>
       <c r="E69" s="2">
-        <v>41501</v>
+        <v>37770</v>
       </c>
       <c r="F69" s="2">
-        <v>45153</v>
+        <v>45075</v>
       </c>
       <c r="G69" t="b">
         <v>0</v>
@@ -3075,22 +3082,22 @@
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
-        <v>410</v>
+        <v>231</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>394</v>
+        <v>409</v>
       </c>
       <c r="C70" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D70">
-        <v>2.375</v>
+        <v>3.25</v>
       </c>
       <c r="E70" s="2">
-        <v>44084</v>
+        <v>41501</v>
       </c>
       <c r="F70" s="2">
-        <v>45179</v>
+        <v>45153</v>
       </c>
       <c r="G70" t="b">
         <v>0</v>
@@ -3098,19 +3105,22 @@
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>196</v>
+        <v>410</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>394</v>
       </c>
       <c r="C71" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D71">
-        <v>11.375</v>
+        <v>2.375</v>
       </c>
       <c r="E71" s="2">
-        <v>37917</v>
+        <v>44084</v>
       </c>
       <c r="F71" s="2">
-        <v>45222</v>
+        <v>45179</v>
       </c>
       <c r="G71" t="b">
         <v>0</v>
@@ -3118,68 +3128,65 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B72" s="1" t="s">
-        <v>11</v>
+        <v>196</v>
       </c>
       <c r="C72" t="s">
-        <v>9</v>
+        <v>93</v>
       </c>
       <c r="D72">
-        <v>2.375</v>
+        <v>11.375</v>
       </c>
       <c r="E72" s="2">
-        <v>44264</v>
+        <v>37917</v>
       </c>
       <c r="F72" s="2">
-        <v>45360</v>
+        <v>45222</v>
       </c>
       <c r="G72" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
-        <v>230</v>
+        <v>10</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>227</v>
+        <v>11</v>
       </c>
       <c r="C73" t="s">
-        <v>94</v>
+        <v>9</v>
       </c>
       <c r="D73">
-        <v>6.25</v>
+        <v>2.375</v>
       </c>
       <c r="E73" s="2">
-        <v>43536</v>
+        <v>44264</v>
       </c>
       <c r="F73" s="2">
-        <v>45363</v>
+        <v>45360</v>
       </c>
       <c r="G73" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
-        <v>411</v>
+        <v>230</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>395</v>
+        <v>227</v>
       </c>
       <c r="C74" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D74">
-        <v>4.5</v>
+        <v>6.25</v>
       </c>
       <c r="E74" s="2">
-        <v>42845</v>
+        <v>43536</v>
       </c>
       <c r="F74" s="2">
-        <v>45402</v>
+        <v>45363</v>
       </c>
       <c r="G74" t="b">
         <v>0</v>
@@ -3187,19 +3194,22 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
-        <v>197</v>
+        <v>411</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>395</v>
       </c>
       <c r="C75" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D75">
-        <v>12.375</v>
+        <v>4.5</v>
       </c>
       <c r="E75" s="2">
-        <v>38141</v>
+        <v>42845</v>
       </c>
       <c r="F75" s="2">
-        <v>45446</v>
+        <v>45402</v>
       </c>
       <c r="G75" t="b">
         <v>0</v>
@@ -3207,19 +3217,19 @@
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C76" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D76">
-        <v>12.875</v>
+        <v>12.375</v>
       </c>
       <c r="E76" s="2">
-        <v>38204</v>
+        <v>38141</v>
       </c>
       <c r="F76" s="2">
-        <v>45509</v>
+        <v>45446</v>
       </c>
       <c r="G76" t="b">
         <v>0</v>
@@ -3227,19 +3237,19 @@
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C77" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D77">
-        <v>4.125</v>
+        <v>12.875</v>
       </c>
       <c r="E77" s="2">
-        <v>41871</v>
+        <v>38204</v>
       </c>
       <c r="F77" s="2">
-        <v>45524</v>
+        <v>45509</v>
       </c>
       <c r="G77" t="b">
         <v>0</v>
@@ -3247,22 +3257,19 @@
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
-        <v>412</v>
-      </c>
-      <c r="B78" s="1" t="s">
-        <v>396</v>
+        <v>199</v>
       </c>
       <c r="C78" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D78">
-        <v>4.25</v>
+        <v>4.125</v>
       </c>
       <c r="E78" s="2">
-        <v>43755</v>
+        <v>41871</v>
       </c>
       <c r="F78" s="2">
-        <v>45582</v>
+        <v>45524</v>
       </c>
       <c r="G78" t="b">
         <v>0</v>
@@ -3270,19 +3277,22 @@
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
-        <v>200</v>
+        <v>412</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>396</v>
       </c>
       <c r="C79" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D79">
-        <v>13.75</v>
+        <v>4.25</v>
       </c>
       <c r="E79" s="2">
-        <v>38302</v>
+        <v>43755</v>
       </c>
       <c r="F79" s="2">
-        <v>45607</v>
+        <v>45582</v>
       </c>
       <c r="G79" t="b">
         <v>0</v>
@@ -3290,22 +3300,19 @@
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
-        <v>413</v>
-      </c>
-      <c r="B80" s="1" t="s">
-        <v>397</v>
+        <v>200</v>
       </c>
       <c r="C80" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D80">
-        <v>5.75</v>
+        <v>13.75</v>
       </c>
       <c r="E80" s="2">
-        <v>43202</v>
+        <v>38302</v>
       </c>
       <c r="F80" s="2">
-        <v>45759</v>
+        <v>45607</v>
       </c>
       <c r="G80" t="b">
         <v>0</v>
@@ -3313,19 +3320,22 @@
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
-        <v>201</v>
+        <v>413</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>397</v>
       </c>
       <c r="C81" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D81">
-        <v>12.125</v>
+        <v>5.75</v>
       </c>
       <c r="E81" s="2">
-        <v>38456</v>
+        <v>43202</v>
       </c>
       <c r="F81" s="2">
-        <v>45761</v>
+        <v>45759</v>
       </c>
       <c r="G81" t="b">
         <v>0</v>
@@ -3333,42 +3343,42 @@
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B82" s="1" t="s">
-        <v>4</v>
+        <v>201</v>
       </c>
       <c r="C82" t="s">
-        <v>12</v>
+        <v>102</v>
       </c>
       <c r="D82">
-        <v>2.625</v>
+        <v>12.125</v>
       </c>
       <c r="E82" s="2">
-        <v>44055</v>
+        <v>38456</v>
       </c>
       <c r="F82" s="2">
-        <v>45881</v>
+        <v>45761</v>
       </c>
       <c r="G82" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
-        <v>27</v>
+        <v>3</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="C83" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="D83">
-        <v>3.625</v>
+        <v>2.625</v>
       </c>
       <c r="E83" s="2">
-        <v>42256</v>
+        <v>44055</v>
       </c>
       <c r="F83" s="2">
-        <v>45909</v>
+        <v>45881</v>
       </c>
       <c r="G83" t="b">
         <v>1</v>
@@ -3376,39 +3386,39 @@
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
-        <v>202</v>
+        <v>27</v>
       </c>
       <c r="C84" t="s">
-        <v>103</v>
+        <v>28</v>
       </c>
       <c r="D84">
-        <v>12.125</v>
+        <v>3.625</v>
       </c>
       <c r="E84" s="2">
-        <v>38645</v>
+        <v>42256</v>
       </c>
       <c r="F84" s="2">
-        <v>45950</v>
+        <v>45909</v>
       </c>
       <c r="G84" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
-        <v>193</v>
+        <v>202</v>
       </c>
       <c r="C85" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D85">
-        <v>18.25</v>
+        <v>12.125</v>
       </c>
       <c r="E85" s="2">
-        <v>36859</v>
+        <v>38645</v>
       </c>
       <c r="F85" s="2">
-        <v>45990</v>
+        <v>45950</v>
       </c>
       <c r="G85" t="b">
         <v>0</v>
@@ -3416,19 +3426,19 @@
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
       <c r="C86" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D86">
-        <v>10.25</v>
+        <v>18.25</v>
       </c>
       <c r="E86" s="2">
-        <v>38736</v>
+        <v>36859</v>
       </c>
       <c r="F86" s="2">
-        <v>46041</v>
+        <v>45990</v>
       </c>
       <c r="G86" t="b">
         <v>0</v>
@@ -3436,45 +3446,42 @@
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B87" s="1" t="s">
-        <v>26</v>
+        <v>203</v>
       </c>
       <c r="C87" t="s">
-        <v>24</v>
+        <v>105</v>
       </c>
       <c r="D87">
-        <v>6.25</v>
+        <v>10.25</v>
       </c>
       <c r="E87" s="2">
-        <v>43510</v>
+        <v>38736</v>
       </c>
       <c r="F87" s="2">
-        <v>46067</v>
+        <v>46041</v>
       </c>
       <c r="G87" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="C88" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="D88">
-        <v>3.375</v>
+        <v>6.25</v>
       </c>
       <c r="E88" s="2">
-        <v>44294</v>
+        <v>43510</v>
       </c>
       <c r="F88" s="2">
-        <v>46120</v>
+        <v>46067</v>
       </c>
       <c r="G88" t="b">
         <v>1</v>
@@ -3482,45 +3489,45 @@
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
-        <v>414</v>
+        <v>0</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>415</v>
+        <v>2</v>
       </c>
       <c r="C89" t="s">
-        <v>106</v>
+        <v>7</v>
       </c>
       <c r="D89">
-        <v>3.5</v>
+        <v>3.375</v>
       </c>
       <c r="E89" s="2">
-        <v>42633</v>
+        <v>44294</v>
       </c>
       <c r="F89" s="2">
-        <v>46285</v>
+        <v>46120</v>
       </c>
       <c r="G89" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
-        <v>237</v>
+        <v>414</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C90" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D90">
-        <v>6.25</v>
+        <v>3.5</v>
       </c>
       <c r="E90" s="2">
-        <v>40836</v>
+        <v>42633</v>
       </c>
       <c r="F90" s="2">
-        <v>46315</v>
+        <v>46285</v>
       </c>
       <c r="G90" t="b">
         <v>0</v>
@@ -3528,19 +3535,22 @@
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
-        <v>204</v>
+        <v>237</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>416</v>
       </c>
       <c r="C91" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D91">
-        <v>8</v>
+        <v>6.25</v>
       </c>
       <c r="E91" s="2">
-        <v>39058</v>
+        <v>40836</v>
       </c>
       <c r="F91" s="2">
-        <v>46363</v>
+        <v>46315</v>
       </c>
       <c r="G91" t="b">
         <v>0</v>
@@ -3548,22 +3558,19 @@
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="B92" s="1" t="s">
-        <v>417</v>
+        <v>204</v>
       </c>
       <c r="C92" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D92">
-        <v>5.375</v>
+        <v>8</v>
       </c>
       <c r="E92" s="2">
-        <v>40969</v>
+        <v>39058</v>
       </c>
       <c r="F92" s="2">
-        <v>46447</v>
+        <v>46363</v>
       </c>
       <c r="G92" t="b">
         <v>0</v>
@@ -3571,19 +3578,22 @@
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
-        <v>1</v>
+        <v>236</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>417</v>
       </c>
       <c r="C93" t="s">
-        <v>8</v>
+        <v>109</v>
       </c>
       <c r="D93">
-        <v>4.75</v>
+        <v>5.375</v>
       </c>
       <c r="E93" s="2">
-        <v>42859</v>
+        <v>40969</v>
       </c>
       <c r="F93" s="2">
-        <v>46511</v>
+        <v>46447</v>
       </c>
       <c r="G93" t="b">
         <v>0</v>
@@ -3591,62 +3601,62 @@
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="B94" s="1" t="s">
-        <v>240</v>
+        <v>1</v>
       </c>
       <c r="C94" t="s">
-        <v>239</v>
+        <v>8</v>
       </c>
       <c r="D94">
-        <v>4.625</v>
+        <v>4.75</v>
       </c>
       <c r="E94" s="2">
-        <v>44532</v>
+        <v>42859</v>
       </c>
       <c r="F94" s="2">
-        <v>46540</v>
+        <v>46511</v>
       </c>
       <c r="G94" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
-        <v>205</v>
+        <v>238</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>240</v>
       </c>
       <c r="C95" t="s">
-        <v>110</v>
+        <v>239</v>
       </c>
       <c r="D95">
-        <v>8.625</v>
+        <v>4.625</v>
       </c>
       <c r="E95" s="2">
-        <v>39331</v>
+        <v>44532</v>
       </c>
       <c r="F95" s="2">
-        <v>46636</v>
+        <v>46540</v>
       </c>
       <c r="G95" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C96" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D96">
-        <v>6.25</v>
+        <v>8.625</v>
       </c>
       <c r="E96" s="2">
-        <v>43181</v>
+        <v>39331</v>
       </c>
       <c r="F96" s="2">
-        <v>46834</v>
+        <v>46636</v>
       </c>
       <c r="G96" t="b">
         <v>0</v>
@@ -3654,45 +3664,42 @@
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B97" s="1" t="s">
-        <v>15</v>
+        <v>206</v>
       </c>
       <c r="C97" t="s">
-        <v>16</v>
+        <v>111</v>
       </c>
       <c r="D97">
-        <v>3.625</v>
+        <v>6.25</v>
       </c>
       <c r="E97" s="2">
-        <v>44308</v>
+        <v>43181</v>
       </c>
       <c r="F97" s="2">
-        <v>46865</v>
+        <v>46834</v>
       </c>
       <c r="G97" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C98" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D98">
-        <v>3.75</v>
+        <v>3.625</v>
       </c>
       <c r="E98" s="2">
-        <v>44420</v>
+        <v>44308</v>
       </c>
       <c r="F98" s="2">
-        <v>46977</v>
+        <v>46865</v>
       </c>
       <c r="G98" t="b">
         <v>1</v>
@@ -3700,39 +3707,42 @@
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
-        <v>207</v>
+        <v>18</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="C99" t="s">
-        <v>112</v>
+        <v>17</v>
       </c>
       <c r="D99">
-        <v>9.5</v>
+        <v>3.75</v>
       </c>
       <c r="E99" s="2">
-        <v>39786</v>
+        <v>44420</v>
       </c>
       <c r="F99" s="2">
-        <v>47091</v>
+        <v>46977</v>
       </c>
       <c r="G99" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C100" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D100">
-        <v>6.875</v>
+        <v>9.5</v>
       </c>
       <c r="E100" s="2">
-        <v>43475</v>
+        <v>39786</v>
       </c>
       <c r="F100" s="2">
-        <v>47128</v>
+        <v>47091</v>
       </c>
       <c r="G100" t="b">
         <v>0</v>
@@ -3740,19 +3750,19 @@
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C101" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D101">
-        <v>8.75</v>
+        <v>6.875</v>
       </c>
       <c r="E101" s="2">
-        <v>40325</v>
+        <v>43475</v>
       </c>
       <c r="F101" s="2">
-        <v>47630</v>
+        <v>47128</v>
       </c>
       <c r="G101" t="b">
         <v>0</v>
@@ -3760,19 +3770,19 @@
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
-        <v>22</v>
+        <v>209</v>
       </c>
       <c r="C102" t="s">
-        <v>21</v>
+        <v>114</v>
       </c>
       <c r="D102">
-        <v>2.875</v>
+        <v>8.75</v>
       </c>
       <c r="E102" s="2">
-        <v>44021</v>
+        <v>40325</v>
       </c>
       <c r="F102" s="2">
-        <v>47673</v>
+        <v>47630</v>
       </c>
       <c r="G102" t="b">
         <v>0</v>
@@ -3780,19 +3790,19 @@
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
-        <v>210</v>
+        <v>22</v>
       </c>
       <c r="C103" t="s">
-        <v>115</v>
+        <v>21</v>
       </c>
       <c r="D103">
-        <v>12.5</v>
+        <v>2.875</v>
       </c>
       <c r="E103" s="2">
-        <v>38561</v>
+        <v>44021</v>
       </c>
       <c r="F103" s="2">
-        <v>47692</v>
+        <v>47673</v>
       </c>
       <c r="G103" t="b">
         <v>0</v>
@@ -3800,19 +3810,19 @@
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C104" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D104">
-        <v>11.25</v>
+        <v>12.5</v>
       </c>
       <c r="E104" s="2">
-        <v>38743</v>
+        <v>38561</v>
       </c>
       <c r="F104" s="2">
-        <v>47874</v>
+        <v>47692</v>
       </c>
       <c r="G104" t="b">
         <v>0</v>
@@ -3820,19 +3830,19 @@
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C105" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D105">
-        <v>8</v>
+        <v>11.25</v>
       </c>
       <c r="E105" s="2">
-        <v>40743</v>
+        <v>38743</v>
       </c>
       <c r="F105" s="2">
-        <v>48048</v>
+        <v>47874</v>
       </c>
       <c r="G105" t="b">
         <v>0</v>
@@ -3840,59 +3850,59 @@
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
-        <v>20</v>
+        <v>212</v>
       </c>
       <c r="C106" t="s">
-        <v>23</v>
+        <v>117</v>
       </c>
       <c r="D106">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E106" s="2">
-        <v>44399</v>
+        <v>40743</v>
       </c>
       <c r="F106" s="2">
-        <v>48051</v>
+        <v>48048</v>
       </c>
       <c r="G106" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
-        <v>213</v>
+        <v>20</v>
       </c>
       <c r="C107" t="s">
-        <v>118</v>
+        <v>23</v>
       </c>
       <c r="D107">
-        <v>9.375</v>
+        <v>4</v>
       </c>
       <c r="E107" s="2">
-        <v>38995</v>
+        <v>44399</v>
       </c>
       <c r="F107" s="2">
-        <v>48126</v>
+        <v>48051</v>
       </c>
       <c r="G107" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C108" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D108">
-        <v>5.875</v>
+        <v>9.375</v>
       </c>
       <c r="E108" s="2">
-        <v>40941</v>
+        <v>38995</v>
       </c>
       <c r="F108" s="2">
-        <v>48246</v>
+        <v>48126</v>
       </c>
       <c r="G108" t="b">
         <v>0</v>
@@ -3900,22 +3910,19 @@
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="B109" s="1" t="s">
-        <v>418</v>
+        <v>214</v>
       </c>
       <c r="C109" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D109">
         <v>5.875</v>
       </c>
       <c r="E109" s="2">
-        <v>40969</v>
+        <v>40941</v>
       </c>
       <c r="F109" s="2">
-        <v>48274</v>
+        <v>48246</v>
       </c>
       <c r="G109" t="b">
         <v>0</v>
@@ -3923,19 +3930,22 @@
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
-        <v>215</v>
+        <v>234</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>418</v>
       </c>
       <c r="C110" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D110">
-        <v>5.75</v>
+        <v>5.875</v>
       </c>
       <c r="E110" s="2">
-        <v>41179</v>
+        <v>40969</v>
       </c>
       <c r="F110" s="2">
-        <v>48484</v>
+        <v>48274</v>
       </c>
       <c r="G110" t="b">
         <v>0</v>
@@ -3943,19 +3953,19 @@
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C111" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D111">
-        <v>8.5</v>
+        <v>5.75</v>
       </c>
       <c r="E111" s="2">
-        <v>39415</v>
+        <v>41179</v>
       </c>
       <c r="F111" s="2">
-        <v>48547</v>
+        <v>48484</v>
       </c>
       <c r="G111" t="b">
         <v>0</v>
@@ -3963,19 +3973,19 @@
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C112" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D112">
-        <v>3.625</v>
+        <v>8.5</v>
       </c>
       <c r="E112" s="2">
-        <v>41354</v>
+        <v>39415</v>
       </c>
       <c r="F112" s="2">
-        <v>48659</v>
+        <v>48547</v>
       </c>
       <c r="G112" t="b">
         <v>0</v>
@@ -3983,19 +3993,19 @@
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C113" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D113">
-        <v>9.25</v>
+        <v>3.625</v>
       </c>
       <c r="E113" s="2">
-        <v>40122</v>
+        <v>41354</v>
       </c>
       <c r="F113" s="2">
-        <v>49253</v>
+        <v>48659</v>
       </c>
       <c r="G113" t="b">
         <v>0</v>
@@ -4003,19 +4013,19 @@
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C114" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D114">
-        <v>8</v>
+        <v>9.25</v>
       </c>
       <c r="E114" s="2">
-        <v>40451</v>
+        <v>40122</v>
       </c>
       <c r="F114" s="2">
-        <v>49582</v>
+        <v>49253</v>
       </c>
       <c r="G114" t="b">
         <v>0</v>
@@ -4023,19 +4033,19 @@
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C115" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D115">
-        <v>8.125</v>
+        <v>8</v>
       </c>
       <c r="E115" s="2">
-        <v>40528</v>
+        <v>40451</v>
       </c>
       <c r="F115" s="2">
-        <v>49659</v>
+        <v>49582</v>
       </c>
       <c r="G115" t="b">
         <v>0</v>
@@ -4043,19 +4053,19 @@
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C116" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D116">
-        <v>7.625</v>
+        <v>8.125</v>
       </c>
       <c r="E116" s="2">
-        <v>40815</v>
+        <v>40528</v>
       </c>
       <c r="F116" s="2">
-        <v>49947</v>
+        <v>49659</v>
       </c>
       <c r="G116" t="b">
         <v>0</v>
@@ -4063,19 +4073,19 @@
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C117" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D117">
-        <v>5.25</v>
+        <v>7.625</v>
       </c>
       <c r="E117" s="2">
-        <v>42873</v>
+        <v>40815</v>
       </c>
       <c r="F117" s="2">
-        <v>50178</v>
+        <v>49947</v>
       </c>
       <c r="G117" t="b">
         <v>0</v>
@@ -4083,19 +4093,19 @@
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C118" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D118">
-        <v>5.75</v>
+        <v>5.25</v>
       </c>
       <c r="E118" s="2">
-        <v>41137</v>
+        <v>42873</v>
       </c>
       <c r="F118" s="2">
-        <v>50268</v>
+        <v>50178</v>
       </c>
       <c r="G118" t="b">
         <v>0</v>
@@ -4103,22 +4113,19 @@
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="B119" s="1" t="s">
-        <v>419</v>
+        <v>223</v>
       </c>
       <c r="C119" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D119">
-        <v>6.125</v>
+        <v>5.75</v>
       </c>
       <c r="E119" s="2">
-        <v>41206</v>
+        <v>41137</v>
       </c>
       <c r="F119" s="2">
-        <v>50337</v>
+        <v>50268</v>
       </c>
       <c r="G119" t="b">
         <v>0</v>
@@ -4126,19 +4133,22 @@
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
-        <v>224</v>
+        <v>235</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>419</v>
       </c>
       <c r="C120" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D120">
-        <v>6.5</v>
+        <v>6.125</v>
       </c>
       <c r="E120" s="2">
-        <v>43153</v>
+        <v>41206</v>
       </c>
       <c r="F120" s="2">
-        <v>50458</v>
+        <v>50337</v>
       </c>
       <c r="G120" t="b">
         <v>0</v>
@@ -4146,19 +4156,19 @@
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C121" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D121">
-        <v>6.75</v>
+        <v>6.5</v>
       </c>
       <c r="E121" s="2">
-        <v>43489</v>
+        <v>43153</v>
       </c>
       <c r="F121" s="2">
-        <v>50794</v>
+        <v>50458</v>
       </c>
       <c r="G121" t="b">
         <v>0</v>
@@ -4166,19 +4176,19 @@
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C122" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D122">
-        <v>4.625</v>
+        <v>6.75</v>
       </c>
       <c r="E122" s="2">
-        <v>42256</v>
+        <v>43489</v>
       </c>
       <c r="F122" s="2">
-        <v>51388</v>
+        <v>50794</v>
       </c>
       <c r="G122" t="b">
         <v>0</v>
@@ -4186,21 +4196,41 @@
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="C123" t="s">
+        <v>133</v>
+      </c>
+      <c r="D123">
+        <v>4.625</v>
+      </c>
+      <c r="E123" s="2">
+        <v>42256</v>
+      </c>
+      <c r="F123" s="2">
+        <v>51388</v>
+      </c>
+      <c r="G123" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A124" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="C123" t="s">
+      <c r="C124" t="s">
         <v>134</v>
       </c>
-      <c r="D123">
+      <c r="D124">
         <v>5.125</v>
       </c>
-      <c r="E123" s="2">
+      <c r="E124" s="2">
         <v>44392</v>
       </c>
-      <c r="F123" s="2">
+      <c r="F124" s="2">
         <v>51697</v>
       </c>
-      <c r="G123" t="b">
+      <c r="G124" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>